<commit_message>
Fixed CDS phs002293 TC04 and TC05
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC04_CDS_phs002293_SampleTumorStatus_Normal.xlsx
+++ b/InputFiles/CDS/TC04_CDS_phs002293_SampleTumorStatus_Normal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0305\Commons_Automation\InputFiles\CDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/04-15-2025/Commons_Automation/InputFiles/CDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34753441-3846-4D97-882D-A837F48C7463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D7CFDB-C681-8140-9F50-87A5DC7DB227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="38820" yWindow="-1680" windowWidth="33480" windowHeight="24420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,53 +110,6 @@
     df_genomic_info gi ON gi."file.file_id" = f.file_id
 WHERE 
       s.phs_accession = 'phs002293' AND smp.sample_tumor_status = 'Normal';</t>
-  </si>
-  <si>
-    <t>SELECT
-    f1.file_name AS "File Name",
-    s.study_name AS "Study Name",
-    s.phs_accession AS "Accession",
-    sp.participant_id AS "Participant Id",
-    COALESCE((
-        SELECT
-            REPLACE(GROUP_CONCAT(CASE WHEN rn &lt;= 5 THEN smp.sample_id ELSE NULL END, ', '), ', , ', ', ') ||
-            CASE WHEN MAX(rn) &gt; 5 THEN ', ...' ELSE '' END
-        FROM (
-            SELECT
-                smp.sample_id,
-                ROW_NUMBER() OVER (ORDER BY smp.sample_id) AS rn
-            FROM df_sample smp
-            WHERE smp."participant.study_participant_id" = sp.study_participant_id
-        ) smp
-    ), '') AS "Sample Id",
-    f1.file_type AS "File Type",
-    gi.library_strategy AS "Library Strategy"
-FROM 
-    df_study s
-INNER JOIN 
-    df_participant sp ON sp."study.phs_accession" = s.phs_accession
-INNER JOIN  
-    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
-INNER JOIN 
-    df_file f1 ON f1."participant.study_participant_id" = sp.study_participant_id
-INNER JOIN
-    df_genomic_info gi ON gi."file.file_id" = f1.file_id
-INNER JOIN
-    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
-INNER JOIN
-    df_program p ON p.program_acronym = s."program.program_acronym"
-WHERE 
-     s.phs_accession = 'phs002293' AND smp.sample_tumor_status = 'Normal'
-GROUP BY
-    f1.file_name,
-    s.study_name,
-    s.phs_accession,
-    sp.participant_id,
-    f1.file_type,
-    gi.library_strategy
-ORDER BY 
-    f1.file_name ASC
---LIMIT 100;</t>
   </si>
   <si>
     <t>WITH 
@@ -224,14 +177,68 @@
     gender
 LIMIT 100;</t>
   </si>
+  <si>
+    <t>SELECT
+    f1.file_name AS "File Name",
+    s.study_name AS "Study Name",
+    s.phs_accession AS "Accession",
+    sp.participant_id AS "Participant Id",
+    COALESCE((
+        SELECT
+            REPLACE(GROUP_CONCAT(CASE WHEN rn &lt;= 5 THEN smp.sample_id ELSE NULL END, ', '), ', , ', ', ') ||
+            CASE WHEN MAX(rn) &gt; 5 THEN ', ...' ELSE '' END
+        FROM (
+            SELECT
+                smp.sample_id,
+                ROW_NUMBER() OVER (ORDER BY smp.sample_id) AS rn
+            FROM df_sample smp
+            WHERE smp."participant.study_participant_id" = sp.study_participant_id
+        ) smp
+    ), '') AS "Sample Id",
+    f1.file_type AS "File Type",
+    gi.library_strategy AS "Library Strategy"
+FROM 
+    df_study s
+INNER JOIN 
+    df_participant sp ON sp."study.phs_accession" = s.phs_accession
+INNER JOIN  
+    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+INNER JOIN 
+    df_file f1 ON f1."participant.study_participant_id" = sp.study_participant_id
+INNER JOIN
+    df_genomic_info gi ON gi."file.file_id" = f1.file_id
+INNER JOIN
+    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+INNER JOIN
+    df_program p ON p.program_acronym = s."program.program_acronym"
+WHERE 
+     s.phs_accession = 'phs002293' AND smp.sample_tumor_status = 'Normal'
+GROUP BY
+    f1.file_name,
+    s.study_name,
+    s.phs_accession,
+    sp.participant_id,
+    f1.file_type,
+    gi.library_strategy
+ORDER BY 
+    f1.file_name ASC
+LIMIT 100;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -284,14 +291,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -614,19 +624,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.140625" customWidth="1"/>
-    <col min="5" max="5" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.83203125" customWidth="1"/>
+    <col min="4" max="4" width="70.1640625" customWidth="1"/>
+    <col min="5" max="5" width="63.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -643,12 +653,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
@@ -660,7 +670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -669,24 +679,24 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>